<commit_message>
Début validation des ressources
</commit_message>
<xml_diff>
--- a/Documentation/Menu.xlsx
+++ b/Documentation/Menu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dbfe86086311eed9/ProjectPlan/ProjectPlan/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Marcel\Repos\ProjectPlan2\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="8_{FEC3D0D4-2056-4A06-9277-4264D18D2125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C83815F0-D82B-492C-8644-3BD21D9E99E4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6561D9-C0F5-4801-8C6A-FD5A0BA38D6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{F6C78DB4-3C60-4F3C-8401-DD6D1D9E0A76}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F6C78DB4-3C60-4F3C-8401-DD6D1D9E0A76}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -184,13 +184,7 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -198,7 +192,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE03541-3CE3-4E6D-A934-050911ECF6BD}">
   <dimension ref="C3:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B901C4AD-3069-496F-9D65-13B52BF9CD80}">
   <dimension ref="D6:AB40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
@@ -612,699 +612,699 @@
   </cols>
   <sheetData>
     <row r="6" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4" t="s">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4" t="s">
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="4"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
     </row>
     <row r="7" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <v>8</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="4">
         <v>9</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="4">
         <v>10</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="4">
         <v>11</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="4">
         <v>13</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="4">
         <v>14</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="4">
         <v>15</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="4">
         <v>16</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="4">
         <v>8</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="4">
         <v>9</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="4">
         <v>10</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="4">
         <v>11</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="4">
         <v>13</v>
       </c>
-      <c r="R7" s="6">
+      <c r="R7" s="4">
         <v>14</v>
       </c>
-      <c r="S7" s="6">
+      <c r="S7" s="4">
         <v>15</v>
       </c>
-      <c r="T7" s="6">
+      <c r="T7" s="4">
         <v>16</v>
       </c>
-      <c r="U7" s="6">
+      <c r="U7" s="4">
         <v>8</v>
       </c>
-      <c r="V7" s="6">
+      <c r="V7" s="4">
         <v>9</v>
       </c>
-      <c r="W7" s="6">
+      <c r="W7" s="4">
         <v>10</v>
       </c>
-      <c r="X7" s="6">
+      <c r="X7" s="4">
         <v>11</v>
       </c>
-      <c r="Y7" s="6">
+      <c r="Y7" s="4">
         <v>13</v>
       </c>
-      <c r="Z7" s="6">
+      <c r="Z7" s="4">
         <v>14</v>
       </c>
-      <c r="AA7" s="6">
+      <c r="AA7" s="4">
         <v>15</v>
       </c>
-      <c r="AB7" s="6">
+      <c r="AB7" s="4">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
     </row>
     <row r="9" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
     </row>
     <row r="10" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
     </row>
     <row r="11" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="3"/>
-      <c r="AB11" s="3"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
     </row>
     <row r="16" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2" t="s">
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2" t="s">
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2" t="s">
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
     </row>
     <row r="17" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="3">
         <v>8</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
     </row>
     <row r="18" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D18" s="7"/>
-      <c r="E18" s="5">
+      <c r="D18" s="6"/>
+      <c r="E18" s="3">
         <v>9</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
     </row>
     <row r="19" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D19" s="7"/>
-      <c r="E19" s="5">
+      <c r="D19" s="6"/>
+      <c r="E19" s="3">
         <v>10</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
     </row>
     <row r="20" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D20" s="7"/>
-      <c r="E20" s="5">
+      <c r="D20" s="6"/>
+      <c r="E20" s="3">
         <v>11</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
     </row>
     <row r="21" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D21" s="7"/>
-      <c r="E21" s="5">
+      <c r="D21" s="6"/>
+      <c r="E21" s="3">
         <v>13</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
     </row>
     <row r="22" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D22" s="7"/>
-      <c r="E22" s="5">
+      <c r="D22" s="6"/>
+      <c r="E22" s="3">
         <v>14</v>
       </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
     </row>
     <row r="23" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D23" s="7"/>
-      <c r="E23" s="5">
+      <c r="D23" s="6"/>
+      <c r="E23" s="3">
         <v>15</v>
       </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
     </row>
     <row r="24" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D24" s="7"/>
-      <c r="E24" s="5">
+      <c r="D24" s="6"/>
+      <c r="E24" s="3">
         <v>16</v>
       </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
     </row>
     <row r="25" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="3">
         <v>8</v>
       </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
     </row>
     <row r="26" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D26" s="7"/>
-      <c r="E26" s="5">
+      <c r="D26" s="6"/>
+      <c r="E26" s="3">
         <v>9</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
     </row>
     <row r="27" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D27" s="7"/>
-      <c r="E27" s="5">
+      <c r="D27" s="6"/>
+      <c r="E27" s="3">
         <v>10</v>
       </c>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
     </row>
     <row r="28" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D28" s="7"/>
-      <c r="E28" s="5">
+      <c r="D28" s="6"/>
+      <c r="E28" s="3">
         <v>11</v>
       </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
     </row>
     <row r="29" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D29" s="7"/>
-      <c r="E29" s="5">
+      <c r="D29" s="6"/>
+      <c r="E29" s="3">
         <v>13</v>
       </c>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
     </row>
     <row r="30" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D30" s="7"/>
-      <c r="E30" s="5">
+      <c r="D30" s="6"/>
+      <c r="E30" s="3">
         <v>14</v>
       </c>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
     </row>
     <row r="31" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D31" s="7"/>
-      <c r="E31" s="5">
+      <c r="D31" s="6"/>
+      <c r="E31" s="3">
         <v>15</v>
       </c>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
     </row>
     <row r="32" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D32" s="7"/>
-      <c r="E32" s="5">
+      <c r="D32" s="6"/>
+      <c r="E32" s="3">
         <v>16</v>
       </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
     </row>
     <row r="33" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="3">
         <v>8</v>
       </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
     </row>
     <row r="34" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D34" s="7"/>
-      <c r="E34" s="5">
+      <c r="D34" s="6"/>
+      <c r="E34" s="3">
         <v>9</v>
       </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
     </row>
     <row r="35" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D35" s="7"/>
-      <c r="E35" s="5">
+      <c r="D35" s="6"/>
+      <c r="E35" s="3">
         <v>10</v>
       </c>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
-      <c r="P35" s="3"/>
-      <c r="Q35" s="3"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
     </row>
     <row r="36" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D36" s="7"/>
-      <c r="E36" s="5">
+      <c r="D36" s="6"/>
+      <c r="E36" s="3">
         <v>11</v>
       </c>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
     </row>
     <row r="37" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D37" s="7"/>
-      <c r="E37" s="5">
+      <c r="D37" s="6"/>
+      <c r="E37" s="3">
         <v>13</v>
       </c>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
     </row>
     <row r="38" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D38" s="7"/>
-      <c r="E38" s="5">
+      <c r="D38" s="6"/>
+      <c r="E38" s="3">
         <v>14</v>
       </c>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
     </row>
     <row r="39" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D39" s="7"/>
-      <c r="E39" s="5">
+      <c r="D39" s="6"/>
+      <c r="E39" s="3">
         <v>15</v>
       </c>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
     </row>
     <row r="40" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D40" s="7"/>
-      <c r="E40" s="5">
+      <c r="D40" s="6"/>
+      <c r="E40" s="3">
         <v>16</v>
       </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D33:D40"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="O16:Q16"/>
     <mergeCell ref="E6:L6"/>
     <mergeCell ref="M6:T6"/>
     <mergeCell ref="U6:AB6"/>
     <mergeCell ref="D17:D24"/>
     <mergeCell ref="D25:D32"/>
-    <mergeCell ref="D33:D40"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="O16:Q16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>